<commit_message>
Last Cross Sections with more couplings
</commit_message>
<xml_diff>
--- a/01_signal_production/Data_Generation_wRHC/Data_5K_13_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
+++ b/01_signal_production/Data_Generation_wRHC/Data_5K_13_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1750</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>2250</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>1750</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>2250</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -488,297 +473,1597 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.0625</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>933.1</v>
+        <v>0.1977</v>
       </c>
       <c r="C2" t="n">
-        <v>19.87</v>
+        <v>0.03314</v>
       </c>
       <c r="D2" t="n">
-        <v>1.531</v>
+        <v>0.006509</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1965</v>
+        <v>0.001419</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03334</v>
+        <v>0.0003284</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00651</v>
+        <v>7.957999999999999e-05</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00142</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0003288</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7.974000000000001e-05</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1.971e-05</v>
+        <v>1.98e-05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.125</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>926.3</v>
+        <v>0.1974</v>
       </c>
       <c r="C3" t="n">
-        <v>19.82</v>
+        <v>0.03313</v>
       </c>
       <c r="D3" t="n">
-        <v>1.52</v>
+        <v>0.006536</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1972</v>
+        <v>0.001419</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03334</v>
+        <v>0.0003283</v>
       </c>
       <c r="G3" t="n">
-        <v>0.006535</v>
+        <v>8.002e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001422</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0003291</v>
-      </c>
-      <c r="J3" t="n">
-        <v>8.006e-05</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1.991e-05</v>
+        <v>1.993e-05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.1875</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>927.2</v>
+        <v>0.1951</v>
       </c>
       <c r="C4" t="n">
-        <v>19.95</v>
+        <v>0.03334</v>
       </c>
       <c r="D4" t="n">
-        <v>1.525</v>
+        <v>0.006537</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1967</v>
+        <v>0.001425</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03332</v>
+        <v>0.0003293</v>
       </c>
       <c r="G4" t="n">
-        <v>0.006506</v>
+        <v>7.949e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001421</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0003298</v>
-      </c>
-      <c r="J4" t="n">
-        <v>7.933e-05</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.997e-05</v>
+        <v>1.992e-05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>937.3</v>
+        <v>0.1953</v>
       </c>
       <c r="C5" t="n">
-        <v>20.04</v>
+        <v>0.03319</v>
       </c>
       <c r="D5" t="n">
-        <v>1.537</v>
+        <v>0.006526</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1974</v>
+        <v>0.001421</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03342</v>
+        <v>0.0003264</v>
       </c>
       <c r="G5" t="n">
-        <v>0.006545</v>
+        <v>7.970999999999999e-05</v>
       </c>
       <c r="H5" t="n">
-        <v>0.001419</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0003294</v>
-      </c>
-      <c r="J5" t="n">
-        <v>8.025999999999999e-05</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1.986e-05</v>
+        <v>1.977e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.3125</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>950.2</v>
+        <v>0.197</v>
       </c>
       <c r="C6" t="n">
-        <v>20.36</v>
+        <v>0.03334</v>
       </c>
       <c r="D6" t="n">
-        <v>1.558</v>
+        <v>0.006534</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2015</v>
+        <v>0.001416</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03389</v>
+        <v>0.000329</v>
       </c>
       <c r="G6" t="n">
-        <v>0.006621</v>
+        <v>7.946e-05</v>
       </c>
       <c r="H6" t="n">
-        <v>0.001444</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0003341</v>
-      </c>
-      <c r="J6" t="n">
-        <v>8.064e-05</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2.003e-05</v>
+        <v>1.982e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>0.375</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>973.4</v>
+        <v>0.1959</v>
       </c>
       <c r="C7" t="n">
-        <v>21.03</v>
+        <v>0.03343</v>
       </c>
       <c r="D7" t="n">
-        <v>1.609</v>
+        <v>0.006553</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2081</v>
+        <v>0.001417</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03505</v>
+        <v>0.0003274</v>
       </c>
       <c r="G7" t="n">
-        <v>0.006831</v>
+        <v>7.923e-05</v>
       </c>
       <c r="H7" t="n">
-        <v>0.001476</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0003421</v>
-      </c>
-      <c r="J7" t="n">
-        <v>8.221e-05</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2.03e-05</v>
+        <v>1.996e-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>0.4375</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1024</v>
+        <v>0.1974</v>
       </c>
       <c r="C8" t="n">
-        <v>22.27</v>
+        <v>0.0332</v>
       </c>
       <c r="D8" t="n">
-        <v>1.713</v>
+        <v>0.006513</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2209</v>
+        <v>0.00142</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0369</v>
+        <v>0.0003291</v>
       </c>
       <c r="G8" t="n">
-        <v>0.007206</v>
+        <v>7.978e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.001553</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0003574</v>
-      </c>
-      <c r="J8" t="n">
-        <v>8.506e-05</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2.096e-05</v>
+        <v>1.987e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1963</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.03324</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.006531</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.001418</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0003288</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7.996e-05</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.99e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>0.5625</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1959</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03343</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.006581</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.001419</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0003287</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.938e-05</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.989e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1958</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.03327</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.006547</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.001419</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0003284</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.962e-05</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.971e-05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>0.6875</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1971</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.03321</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.00656</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.00142</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0003284</v>
+      </c>
+      <c r="G12" t="n">
+        <v>7.964e-05</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.982e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.1977</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.03306</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.006492</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.001409</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0003271</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.949999999999999e-05</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.974e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>0.8125</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.1956</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.03334</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.006507</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.001418</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0003279</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7.965e-05</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.993e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>0.875</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1972</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.03335</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.006521</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.001414</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.000329</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7.956e-05</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.983e-05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>0.9375</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1986</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.03316</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.006524</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.001416</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0003274</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.949e-05</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.973e-05</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1971</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.03339</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.006531</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.00142</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0003264</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7.970999999999999e-05</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.984e-05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>1.0625</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.197</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.03304</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.006536</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.001422</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0003296</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.966000000000001e-05</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.991e-05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>1.125</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1969</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.03331</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.006487</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.001415</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0003279</v>
+      </c>
+      <c r="G19" t="n">
+        <v>7.985e-05</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.995e-05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>1.1875</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1968</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.03326</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.006492</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.001415</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0003299</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.966000000000001e-05</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2.004e-05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1971</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0333</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.006531</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.001418</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0003307</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7.987000000000001e-05</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.986e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>1.3125</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1969</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.03338</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.006494</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.001427</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0003284</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7.981e-05</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.999e-05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>1.375</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.1971</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.03352</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.00652</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.001425</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0003288</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8.012999999999999e-05</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.984e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>1.4375</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1971</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.03342</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00653</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.001424</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0003299</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.981e-05</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.992e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.1987</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.03349</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.006528</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.001418</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0003288</v>
+      </c>
+      <c r="G25" t="n">
+        <v>7.998e-05</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.993e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>1.5625</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1981</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.03343</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.006521</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.001426</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0003289</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7.983999999999999e-05</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.987e-05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>1.625</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.1953</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.03365</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.006569</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.001431</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0003317</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.967e-05</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.987e-05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>1.6875</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1991</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.03351</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.00657</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.001423</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.0003303</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7.957e-05</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.99e-05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.1973</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.03362</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.006542</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.001426</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0003316</v>
+      </c>
+      <c r="G29" t="n">
+        <v>8.01e-05</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.98e-05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>1.8125</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1997</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.03343</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.006573</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.001435</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.0003342</v>
+      </c>
+      <c r="G30" t="n">
+        <v>8.034000000000001e-05</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.997e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>1.875</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.2007</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.03382</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.006584</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.001433</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0003325</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8.03e-05</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2.003e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>1.9375</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.2002</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.03394</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.006604</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.001442</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.0003335</v>
+      </c>
+      <c r="G32" t="n">
+        <v>8.012e-05</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.99e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.2012</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.03371</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.006626</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.001437</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.0003326</v>
+      </c>
+      <c r="G33" t="n">
+        <v>8.041e-05</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2.015e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>2.0625</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.2024</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.03411</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.006673</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.001446</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.0003354</v>
+      </c>
+      <c r="G34" t="n">
+        <v>8.085999999999999e-05</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2.017e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>2.125</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.2016</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.006666</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.001456</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0003357</v>
+      </c>
+      <c r="G35" t="n">
+        <v>8.091e-05</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2.014e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>2.1875</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.2022</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.03403</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.006647</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.001448</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.000336</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8.077e-05</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2.024e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.2032</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.03425</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.00669</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.001447</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.0003376</v>
+      </c>
+      <c r="G37" t="n">
+        <v>8.12e-05</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2.022e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>2.3125</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.2037</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.03444</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.006702</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.001464</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.0003384</v>
+      </c>
+      <c r="G38" t="n">
+        <v>8.148e-05</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2.032e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>2.375</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.2057</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.03447</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.006765</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.001462</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0003375</v>
+      </c>
+      <c r="G39" t="n">
+        <v>8.144000000000001e-05</v>
+      </c>
+      <c r="H39" t="n">
+        <v>2.031e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>2.4375</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.2081</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0348</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.006784</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.001471</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.0003412</v>
+      </c>
+      <c r="G40" t="n">
+        <v>8.213e-05</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2.048e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.2094</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.03486</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.006862</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.001479</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.0003412</v>
+      </c>
+      <c r="G41" t="n">
+        <v>8.203e-05</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2.032e-05</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>2.5625</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.2095</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.03505</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.006865</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.001485</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.000343</v>
+      </c>
+      <c r="G42" t="n">
+        <v>8.295e-05</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2.033e-05</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>2.625</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.2103</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.03542</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.006899</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.0003451</v>
+      </c>
+      <c r="G43" t="n">
+        <v>8.318999999999999e-05</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2.047e-05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>2.6875</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.2118</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.03565</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.006976</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.0003437</v>
+      </c>
+      <c r="G44" t="n">
+        <v>8.299e-05</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2.065e-05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.2122</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.03587</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.006977</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.001514</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.0003505</v>
+      </c>
+      <c r="G45" t="n">
+        <v>8.368999999999999e-05</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2.074e-05</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>2.8125</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.03613</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.007005</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.001509</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.0003503</v>
+      </c>
+      <c r="G46" t="n">
+        <v>8.383e-05</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2.075e-05</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>2.875</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.216</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.03628</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.00703</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.001533</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.0003531</v>
+      </c>
+      <c r="G47" t="n">
+        <v>8.378e-05</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2.079e-05</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>2.9375</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.2195</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.03665</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.007072</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.001546</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.0003548</v>
+      </c>
+      <c r="G48" t="n">
+        <v>8.486e-05</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2.092e-05</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.2197</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.03686</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.007183</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.001546</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.0003569</v>
+      </c>
+      <c r="G49" t="n">
+        <v>8.519e-05</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2.105e-05</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>3.0625</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.2239</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.03718</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.007239</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.001557</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.0003591</v>
+      </c>
+      <c r="G50" t="n">
+        <v>8.558e-05</v>
+      </c>
+      <c r="H50" t="n">
+        <v>2.106e-05</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>3.125</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.2246</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.03762</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.007316</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.001575</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.000363</v>
+      </c>
+      <c r="G51" t="n">
+        <v>8.66e-05</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2.115e-05</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>3.1875</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.03806</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.00735</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.001595</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.0003667</v>
+      </c>
+      <c r="G52" t="n">
+        <v>8.725000000000001e-05</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2.174e-05</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.2303</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.03861</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.007445</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.001609</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.0003685</v>
+      </c>
+      <c r="G53" t="n">
+        <v>8.745e-05</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2.141e-05</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>3.3125</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.2324</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.03885</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.007517</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.001617</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.0003708</v>
+      </c>
+      <c r="G54" t="n">
+        <v>8.841e-05</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2.148e-05</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>3.375</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.2369</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.03965</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.007571</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.001634</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0003726</v>
+      </c>
+      <c r="G55" t="n">
+        <v>8.958000000000001e-05</v>
+      </c>
+      <c r="H55" t="n">
+        <v>2.18e-05</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>3.4375</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.2402</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.03972</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.007743</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.00166</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.0003775</v>
+      </c>
+      <c r="G56" t="n">
+        <v>8.973e-05</v>
+      </c>
+      <c r="H56" t="n">
+        <v>2.176e-05</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
           <t>3.5</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1106</v>
-      </c>
-      <c r="C9" t="n">
-        <v>24.47</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.886</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.243</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.04029</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.007794</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.001677</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0003809</v>
-      </c>
-      <c r="J9" t="n">
-        <v>9.029e-05</v>
-      </c>
-      <c r="K9" t="n">
-        <v>2.195e-05</v>
+      <c r="B57" t="n">
+        <v>0.2423</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.04042</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.00779</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.001679</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.0003825</v>
+      </c>
+      <c r="G57" t="n">
+        <v>9.059e-05</v>
+      </c>
+      <c r="H57" t="n">
+        <v>2.217e-05</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.2009</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.006563</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.001431</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0003319</v>
+      </c>
+      <c r="G58" t="n">
+        <v>8.024e-05</v>
+      </c>
+      <c r="H58" t="n">
+        <v>2.002e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>